<commit_message>
pushing pdf of revised paper
</commit_message>
<xml_diff>
--- a/1b-reps-10-hypothtest.xlsx
+++ b/1b-reps-10-hypothtest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Research-In Review\Baboon FA\BaboonStress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Research-Published\2021-Baboon FA\BaboonStress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15785AFD-2D79-41DC-BD19-D6AC413C21DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08E8AD7-5B9A-4923-B79C-A885967D865D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56450" yWindow="1640" windowWidth="19660" windowHeight="17970" tabRatio="722" xr2:uid="{3123FED7-B888-4F1E-8E92-D9323FB0CFC3}"/>
+    <workbookView xWindow="54060" yWindow="5220" windowWidth="14910" windowHeight="15350" tabRatio="722" xr2:uid="{3123FED7-B888-4F1E-8E92-D9323FB0CFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="FA10" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="46">
   <si>
     <t>M1</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>MXP4_L</t>
+  </si>
+  <si>
+    <t>Teeth</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -557,28 +563,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0D2B6B-8F9B-42F5-A6A5-8DA24D60ACED}">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:I32"/>
+      <selection activeCell="I17" sqref="I16:I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.5234375" defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="14.5" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="1" width="6.3671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7890625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="6.578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.05078125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.68359375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.62890625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.3125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.15625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="6.5234375" style="4"/>
-    <col min="12" max="12" width="6.15625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="6.5234375" style="4"/>
+    <col min="1" max="1" width="6.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.76953125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="6.58984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.04296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.31640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.31640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.1328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.31640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="4"/>
+    <col min="13" max="13" width="6.1328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="6.5" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -603,17 +611,20 @@
       <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="3"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="7"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -621,10 +632,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>20</v>
@@ -633,22 +644,24 @@
         <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="11">
-        <v>8.5620000000000002E-3</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="11">
+        <v>6.2767000000000005E-3</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="8"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -656,10 +669,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>20</v>
@@ -668,22 +681,24 @@
         <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="11">
-        <v>2.8579E-2</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11">
+        <v>1.15709E-2</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="8"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -691,10 +706,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>20</v>
@@ -703,22 +718,24 @@
         <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="11">
-        <v>8.4099999999999991E-3</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1.0606000000000001E-2</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="8"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -726,10 +743,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>20</v>
@@ -738,22 +755,24 @@
         <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="11">
-        <v>1.7562000000000001E-2</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>7.2766999999999997E-3</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="8"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -761,43 +780,45 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="11">
-        <v>3.8048999999999999E-2</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
+        <v>2.3969000000000001E-2</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>20</v>
@@ -806,31 +827,33 @@
         <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="11">
-        <v>2.8692000000000002E-2</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+        <v>25</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>5.0460999999999999E-2</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>20</v>
@@ -844,25 +867,27 @@
       <c r="H8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="11">
-        <v>7.5737000000000013E-2</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="I8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="11">
+        <v>8.5620000000000002E-3</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>20</v>
@@ -876,25 +901,27 @@
       <c r="H9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="11">
-        <v>7.9821000000000003E-2</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="I9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="11">
+        <v>2.8579E-2</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
@@ -903,64 +930,68 @@
         <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="11">
-        <v>6.2767000000000005E-3</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="11">
+        <v>8.4099999999999991E-3</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="11">
-        <v>1.0457000000000001E-2</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="11">
+        <v>1.7562000000000001E-2</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>23</v>
@@ -969,26 +1000,28 @@
         <v>26</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="11">
-        <v>4.4386E-3</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="11">
+        <v>3.8048999999999999E-2</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>20</v>
@@ -997,63 +1030,67 @@
         <v>24</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="11">
-        <v>1.15709E-2</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="11">
+        <v>2.8692000000000002E-2</v>
+      </c>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="11">
-        <v>8.9099999999999995E-3</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="11">
+        <v>7.5737000000000013E-2</v>
+      </c>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A15" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>24</v>
@@ -1062,15 +1099,17 @@
         <v>26</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="11">
-        <v>3.9489999999999997E-2</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="11">
+        <v>7.9821000000000003E-2</v>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1078,16 +1117,16 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>26</v>
@@ -1095,61 +1134,65 @@
       <c r="H16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="11">
-        <v>1.3246999999999998E-2</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="11">
+        <v>1.0457000000000001E-2</v>
+      </c>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="11">
-        <v>1.0606000000000001E-2</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="11">
+        <v>4.4386E-3</v>
+      </c>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>26</v>
@@ -1157,30 +1200,32 @@
       <c r="H18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="11">
-        <v>3.0541000000000002E-2</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="11">
+        <v>8.9099999999999995E-3</v>
+      </c>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>26</v>
@@ -1188,45 +1233,49 @@
       <c r="H19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="11">
-        <v>7.9830000000000005E-3</v>
-      </c>
-      <c r="J19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="11">
+        <v>3.9489999999999997E-2</v>
+      </c>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="11">
-        <v>7.2766999999999997E-3</v>
-      </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="11">
+        <v>1.3246999999999998E-2</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1234,16 +1283,16 @@
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>26</v>
@@ -1251,14 +1300,16 @@
       <c r="H21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I21" s="11">
-        <v>2.0684000000000001E-2</v>
-      </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="11">
+        <v>3.0541000000000002E-2</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1266,16 +1317,16 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>26</v>
@@ -1283,14 +1334,16 @@
       <c r="H22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="11">
-        <v>3.1292E-2</v>
-      </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="11">
+        <v>7.9830000000000005E-3</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1298,13 +1351,13 @@
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>24</v>
@@ -1315,31 +1368,33 @@
       <c r="H23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="11">
-        <v>2.1019000000000003E-2</v>
-      </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="11">
+        <v>2.0684000000000001E-2</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A24" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>26</v>
@@ -1347,46 +1402,51 @@
       <c r="H24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="11">
-        <v>5.5677999999999991E-2</v>
-      </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J24" s="11">
+        <v>3.1292E-2</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A25" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="11">
-        <v>2.3969000000000001E-2</v>
-      </c>
-      <c r="J25" s="2"/>
+      <c r="I25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="11">
+        <v>2.1019000000000003E-2</v>
+      </c>
       <c r="K25" s="2"/>
-      <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="L25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1394,16 +1454,16 @@
         <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>26</v>
@@ -1411,13 +1471,16 @@
       <c r="H26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="11">
-        <v>4.3601999999999995E-2</v>
-      </c>
-      <c r="J26" s="2"/>
-      <c r="M26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="11">
+        <v>5.5677999999999991E-2</v>
+      </c>
+      <c r="K26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1425,13 +1488,13 @@
         <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>24</v>
@@ -1442,12 +1505,15 @@
       <c r="H27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="11">
-        <v>3.9558999999999997E-2</v>
-      </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" s="11">
+        <v>4.3601999999999995E-2</v>
+      </c>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1455,10 +1521,10 @@
         <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>21</v>
@@ -1472,29 +1538,32 @@
       <c r="H28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="11">
-        <v>4.8283E-2</v>
-      </c>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="11">
+        <v>3.9558999999999997E-2</v>
+      </c>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>26</v>
@@ -1502,12 +1571,15 @@
       <c r="H29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="11">
-        <v>6.6650000000000001E-2</v>
-      </c>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J29" s="11">
+        <v>4.8283E-2</v>
+      </c>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -1515,29 +1587,32 @@
         <v>16</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I30" s="11">
-        <v>5.0460999999999999E-2</v>
-      </c>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="I30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J30" s="11">
+        <v>6.6650000000000001E-2</v>
+      </c>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -1562,12 +1637,15 @@
       <c r="H31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="11">
+      <c r="I31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J31" s="11">
         <v>7.0930999999999994E-2</v>
       </c>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -1592,30 +1670,35 @@
       <c r="H32" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I32" s="11">
+      <c r="I32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="11">
         <v>9.9453999999999987E-2</v>
       </c>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="K32" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.7">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="11"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I36" s="1"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.7">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="11"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I37" s="1"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1624,9 +1707,10 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="11"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I38" s="1"/>
+      <c r="J38" s="11"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1635,9 +1719,10 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="11"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I39" s="1"/>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1646,10 +1731,11 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I40" s="1"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1658,10 +1744,11 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I41" s="1"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1670,9 +1757,10 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I42" s="1"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1681,9 +1769,10 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I43" s="1"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1692,9 +1781,10 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I44" s="1"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1703,9 +1793,10 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I45" s="1"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1714,9 +1805,10 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I46" s="1"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1725,9 +1817,10 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="I47" s="1"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1736,8 +1829,9 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1746,8 +1840,9 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1756,9 +1851,10 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="11"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I50" s="1"/>
+      <c r="J50" s="11"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1767,9 +1863,10 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="11"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I51" s="1"/>
+      <c r="J51" s="11"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1778,9 +1875,10 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-      <c r="I52" s="11"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I52" s="1"/>
+      <c r="J52" s="11"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1789,9 +1887,10 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="11"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I53" s="1"/>
+      <c r="J53" s="11"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1800,9 +1899,10 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-      <c r="I54" s="11"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I54" s="1"/>
+      <c r="J54" s="11"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1811,9 +1911,10 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="11"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I55" s="1"/>
+      <c r="J55" s="11"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1822,9 +1923,10 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
-      <c r="I56" s="11"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I56" s="1"/>
+      <c r="J56" s="11"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1833,9 +1935,10 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
-      <c r="I57" s="11"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I57" s="1"/>
+      <c r="J57" s="11"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1844,9 +1947,10 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="11"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I62" s="1"/>
+      <c r="J62" s="11"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1855,9 +1959,10 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="11"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I63" s="1"/>
+      <c r="J63" s="11"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1866,9 +1971,10 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="11"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I64" s="1"/>
+      <c r="J64" s="11"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1877,9 +1983,10 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
-      <c r="I65" s="11"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I65" s="1"/>
+      <c r="J65" s="11"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1888,9 +1995,10 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-      <c r="I66" s="11"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I66" s="1"/>
+      <c r="J66" s="11"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1899,9 +2007,10 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
-      <c r="I67" s="11"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I67" s="1"/>
+      <c r="J67" s="11"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.7">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1910,11 +2019,12 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
-      <c r="I68" s="11"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="11"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I32">
-    <sortCondition ref="H8:H32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J32">
+    <sortCondition ref="G2:G32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>